<commit_message>
added stuff (I forgot what)
</commit_message>
<xml_diff>
--- a/Database/Fabric_Work Order revise new.xlsx
+++ b/Database/Fabric_Work Order revise new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AadeshwarWorkOrder\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD42BD0-0578-4EA2-BBE0-650838B3FB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC16D06-C8F3-467E-9F81-E8ED69A37BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Sheet6" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fabric!$A$1:$N$1153</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fabric!$A$1:$O$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet2!$A$1:$A$857</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet6!$A$1:$C$1100</definedName>
   </definedNames>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12921" uniqueCount="3712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12922" uniqueCount="3713">
   <si>
     <t>SCB</t>
   </si>
@@ -11176,6 +11176,9 @@
   </si>
   <si>
     <t>FN2095550-S-PM9338</t>
+  </si>
+  <si>
+    <t>Dimensions</t>
   </si>
 </sst>
 </file>
@@ -11433,7 +11436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -11511,11 +11514,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11819,9 +11818,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A886" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A902" sqref="A902"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="78" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -11840,7 +11839,8 @@
     <col min="12" max="12" width="18.109375" style="32" customWidth="1"/>
     <col min="13" max="13" width="18.44140625" style="32" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.109375" style="32" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="32"/>
+    <col min="15" max="15" width="13.21875" style="32" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.25">
@@ -11885,6 +11885,9 @@
       </c>
       <c r="N1" s="27" t="s">
         <v>92</v>
+      </c>
+      <c r="O1" s="27" t="s">
+        <v>3712</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -16322,7 +16325,7 @@
       <c r="A128" s="35" t="s">
         <v>2068</v>
       </c>
-      <c r="B128" s="60" t="s">
+      <c r="B128" s="32" t="s">
         <v>2069</v>
       </c>
       <c r="C128" s="35" t="s">
@@ -16356,7 +16359,7 @@
       <c r="A129" s="35" t="s">
         <v>2059</v>
       </c>
-      <c r="B129" s="60" t="s">
+      <c r="B129" s="32" t="s">
         <v>2060</v>
       </c>
       <c r="C129" s="35" t="s">
@@ -16390,7 +16393,7 @@
       <c r="A130" s="35" t="s">
         <v>2074</v>
       </c>
-      <c r="B130" s="60" t="s">
+      <c r="B130" s="32" t="s">
         <v>2075</v>
       </c>
       <c r="C130" s="35" t="s">
@@ -16424,7 +16427,7 @@
       <c r="A131" s="35" t="s">
         <v>1365</v>
       </c>
-      <c r="B131" s="60" t="s">
+      <c r="B131" s="32" t="s">
         <v>1366</v>
       </c>
       <c r="C131" s="35" t="s">
@@ -34931,7 +34934,7 @@
       <c r="A666" s="35" t="s">
         <v>570</v>
       </c>
-      <c r="B666" s="60" t="s">
+      <c r="B666" s="32" t="s">
         <v>571</v>
       </c>
       <c r="C666" s="35" t="s">
@@ -44244,7 +44247,7 @@
       <c r="B935" s="35" t="s">
         <v>3262</v>
       </c>
-      <c r="C935" s="60" t="s">
+      <c r="C935" s="32" t="s">
         <v>3058</v>
       </c>
       <c r="D935" s="35" t="s">
@@ -47098,7 +47101,7 @@
       <c r="B1040" s="35" t="s">
         <v>3247</v>
       </c>
-      <c r="C1040" s="60" t="s">
+      <c r="C1040" s="32" t="s">
         <v>3043</v>
       </c>
       <c r="D1040" s="35" t="s">
@@ -48269,21 +48272,12 @@
       <c r="C1082" s="44" t="s">
         <v>2957</v>
       </c>
-      <c r="D1082" s="60" t="s">
+      <c r="D1082" s="32" t="s">
         <v>3413</v>
       </c>
-      <c r="E1082" s="60" t="s">
+      <c r="E1082" s="32" t="s">
         <v>862</v>
       </c>
-      <c r="F1082" s="61"/>
-      <c r="G1082" s="60"/>
-      <c r="H1082" s="60"/>
-      <c r="I1082" s="60"/>
-      <c r="J1082" s="60"/>
-      <c r="K1082" s="60"/>
-      <c r="L1082" s="60"/>
-      <c r="M1082" s="60"/>
-      <c r="N1082" s="60"/>
     </row>
     <row r="1083" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1083" s="53" t="s">
@@ -48295,21 +48289,12 @@
       <c r="C1083" s="44" t="s">
         <v>3025</v>
       </c>
-      <c r="D1083" s="60" t="s">
+      <c r="D1083" s="32" t="s">
         <v>1117</v>
       </c>
-      <c r="E1083" s="60"/>
-      <c r="F1083" s="61"/>
-      <c r="G1083" s="60"/>
-      <c r="H1083" s="60"/>
-      <c r="I1083" s="60" t="s">
-        <v>133</v>
-      </c>
-      <c r="J1083" s="60"/>
-      <c r="K1083" s="60"/>
-      <c r="L1083" s="60"/>
-      <c r="M1083" s="60"/>
-      <c r="N1083" s="60"/>
+      <c r="I1083" s="32" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="1084" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1084" s="53" t="s">
@@ -48321,21 +48306,12 @@
       <c r="C1084" s="44" t="s">
         <v>2967</v>
       </c>
-      <c r="D1084" s="60" t="s">
+      <c r="D1084" s="32" t="s">
         <v>2715</v>
       </c>
-      <c r="E1084" s="60"/>
-      <c r="F1084" s="61"/>
-      <c r="G1084" s="60"/>
-      <c r="H1084" s="60"/>
-      <c r="I1084" s="60" t="s">
-        <v>133</v>
-      </c>
-      <c r="J1084" s="60"/>
-      <c r="K1084" s="60"/>
-      <c r="L1084" s="60"/>
-      <c r="M1084" s="60"/>
-      <c r="N1084" s="60"/>
+      <c r="I1084" s="32" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="1085" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1085" s="53" t="s">
@@ -48347,21 +48323,12 @@
       <c r="C1085" s="44" t="s">
         <v>3003</v>
       </c>
-      <c r="D1085" s="60" t="s">
+      <c r="D1085" s="32" t="s">
         <v>2715</v>
       </c>
-      <c r="E1085" s="60"/>
-      <c r="F1085" s="61"/>
-      <c r="G1085" s="60"/>
-      <c r="H1085" s="60"/>
-      <c r="I1085" s="60" t="s">
-        <v>133</v>
-      </c>
-      <c r="J1085" s="60"/>
-      <c r="K1085" s="60"/>
-      <c r="L1085" s="60"/>
-      <c r="M1085" s="60"/>
-      <c r="N1085" s="60"/>
+      <c r="I1085" s="32" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="1086" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1086" s="53" t="s">
@@ -48373,21 +48340,12 @@
       <c r="C1086" s="44" t="s">
         <v>3030</v>
       </c>
-      <c r="D1086" s="60" t="s">
+      <c r="D1086" s="32" t="s">
         <v>2715</v>
       </c>
-      <c r="E1086" s="60"/>
-      <c r="F1086" s="61"/>
-      <c r="G1086" s="60"/>
-      <c r="H1086" s="60"/>
-      <c r="I1086" s="60" t="s">
-        <v>133</v>
-      </c>
-      <c r="J1086" s="60"/>
-      <c r="K1086" s="60"/>
-      <c r="L1086" s="60"/>
-      <c r="M1086" s="60"/>
-      <c r="N1086" s="60"/>
+      <c r="I1086" s="32" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="1087" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1087" s="53" t="s">
@@ -48399,21 +48357,12 @@
       <c r="C1087" s="44" t="s">
         <v>2978</v>
       </c>
-      <c r="D1087" s="60" t="s">
+      <c r="D1087" s="32" t="s">
         <v>747</v>
       </c>
-      <c r="E1087" s="60" t="s">
+      <c r="E1087" s="32" t="s">
         <v>1118</v>
       </c>
-      <c r="F1087" s="61"/>
-      <c r="G1087" s="60"/>
-      <c r="H1087" s="60"/>
-      <c r="I1087" s="60"/>
-      <c r="J1087" s="60"/>
-      <c r="K1087" s="60"/>
-      <c r="L1087" s="60"/>
-      <c r="M1087" s="60"/>
-      <c r="N1087" s="60"/>
     </row>
     <row r="1088" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1088" s="53" t="s">
@@ -48425,23 +48374,14 @@
       <c r="C1088" s="44" t="s">
         <v>3054</v>
       </c>
-      <c r="D1088" s="60" t="s">
+      <c r="D1088" s="32" t="s">
         <v>3373</v>
       </c>
-      <c r="E1088" s="60" t="s">
+      <c r="E1088" s="32" t="s">
         <v>857</v>
       </c>
-      <c r="F1088" s="61"/>
-      <c r="G1088" s="60"/>
-      <c r="H1088" s="60"/>
-      <c r="I1088" s="60"/>
-      <c r="J1088" s="60"/>
-      <c r="K1088" s="60"/>
-      <c r="L1088" s="60"/>
-      <c r="M1088" s="60"/>
-      <c r="N1088" s="60"/>
-    </row>
-    <row r="1089" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1089" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1089" s="53" t="s">
         <v>2816</v>
       </c>
@@ -48451,23 +48391,14 @@
       <c r="C1089" s="44" t="s">
         <v>3038</v>
       </c>
-      <c r="D1089" s="60" t="s">
+      <c r="D1089" s="32" t="s">
         <v>1145</v>
       </c>
-      <c r="E1089" s="60" t="s">
+      <c r="E1089" s="32" t="s">
         <v>1118</v>
       </c>
-      <c r="F1089" s="61"/>
-      <c r="G1089" s="60"/>
-      <c r="H1089" s="60"/>
-      <c r="I1089" s="60"/>
-      <c r="J1089" s="60"/>
-      <c r="K1089" s="60"/>
-      <c r="L1089" s="60"/>
-      <c r="M1089" s="60"/>
-      <c r="N1089" s="60"/>
-    </row>
-    <row r="1090" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1090" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1090" s="53" t="s">
         <v>2827</v>
       </c>
@@ -48477,21 +48408,11 @@
       <c r="C1090" s="44" t="s">
         <v>3049</v>
       </c>
-      <c r="D1090" s="60" t="s">
+      <c r="D1090" s="32" t="s">
         <v>3403</v>
       </c>
-      <c r="E1090" s="60"/>
-      <c r="F1090" s="61"/>
-      <c r="G1090" s="60"/>
-      <c r="H1090" s="60"/>
-      <c r="I1090" s="60"/>
-      <c r="J1090" s="60"/>
-      <c r="K1090" s="60"/>
-      <c r="L1090" s="60"/>
-      <c r="M1090" s="60"/>
-      <c r="N1090" s="60"/>
-    </row>
-    <row r="1091" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1091" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1091" s="53" t="s">
         <v>2796</v>
       </c>
@@ -48501,21 +48422,11 @@
       <c r="C1091" s="44" t="s">
         <v>3018</v>
       </c>
-      <c r="D1091" s="60" t="s">
+      <c r="D1091" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="E1091" s="60"/>
-      <c r="F1091" s="61"/>
-      <c r="G1091" s="60"/>
-      <c r="H1091" s="60"/>
-      <c r="I1091" s="60"/>
-      <c r="J1091" s="60"/>
-      <c r="K1091" s="60"/>
-      <c r="L1091" s="60"/>
-      <c r="M1091" s="60"/>
-      <c r="N1091" s="60"/>
-    </row>
-    <row r="1092" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1092" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1092" s="53" t="s">
         <v>2738</v>
       </c>
@@ -48525,25 +48436,17 @@
       <c r="C1092" s="44" t="s">
         <v>2960</v>
       </c>
-      <c r="D1092" s="60" t="s">
+      <c r="D1092" s="32" t="s">
         <v>3403</v>
       </c>
-      <c r="E1092" s="60" t="s">
+      <c r="E1092" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="F1092" s="61"/>
-      <c r="G1092" s="60"/>
-      <c r="H1092" s="60"/>
-      <c r="I1092" s="60" t="s">
-        <v>133</v>
-      </c>
-      <c r="J1092" s="60"/>
-      <c r="K1092" s="60"/>
-      <c r="L1092" s="60"/>
-      <c r="M1092" s="60"/>
-      <c r="N1092" s="60"/>
-    </row>
-    <row r="1093" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I1092" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1093" s="53" t="s">
         <v>2775</v>
       </c>
@@ -48556,20 +48459,11 @@
       <c r="D1093" s="35" t="s">
         <v>3403</v>
       </c>
-      <c r="E1093" s="60" t="s">
+      <c r="E1093" s="32" t="s">
         <v>3416</v>
       </c>
-      <c r="F1093" s="61"/>
-      <c r="G1093" s="60"/>
-      <c r="H1093" s="60"/>
-      <c r="I1093" s="60"/>
-      <c r="J1093" s="60"/>
-      <c r="K1093" s="60"/>
-      <c r="L1093" s="60"/>
-      <c r="M1093" s="60"/>
-      <c r="N1093" s="60"/>
-    </row>
-    <row r="1094" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1094" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1094" s="53" t="s">
         <v>2806</v>
       </c>
@@ -48579,21 +48473,11 @@
       <c r="C1094" s="44" t="s">
         <v>3028</v>
       </c>
-      <c r="D1094" s="60" t="s">
+      <c r="D1094" s="32" t="s">
         <v>517</v>
       </c>
-      <c r="E1094" s="60"/>
-      <c r="F1094" s="61"/>
-      <c r="G1094" s="60"/>
-      <c r="H1094" s="60"/>
-      <c r="I1094" s="60"/>
-      <c r="J1094" s="60"/>
-      <c r="K1094" s="60"/>
-      <c r="L1094" s="60"/>
-      <c r="M1094" s="60"/>
-      <c r="N1094" s="60"/>
-    </row>
-    <row r="1095" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1095" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1095" s="53" t="s">
         <v>2748</v>
       </c>
@@ -48603,23 +48487,14 @@
       <c r="C1095" s="44" t="s">
         <v>2970</v>
       </c>
-      <c r="D1095" s="60" t="s">
+      <c r="D1095" s="32" t="s">
         <v>517</v>
       </c>
-      <c r="E1095" s="60"/>
-      <c r="F1095" s="61"/>
-      <c r="G1095" s="60"/>
-      <c r="H1095" s="60"/>
-      <c r="I1095" s="60" t="s">
-        <v>133</v>
-      </c>
-      <c r="J1095" s="60"/>
-      <c r="K1095" s="60"/>
-      <c r="L1095" s="60"/>
-      <c r="M1095" s="60"/>
-      <c r="N1095" s="60"/>
-    </row>
-    <row r="1096" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I1095" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1096" s="53" t="s">
         <v>2791</v>
       </c>
@@ -48629,23 +48504,14 @@
       <c r="C1096" s="44" t="s">
         <v>3013</v>
       </c>
-      <c r="D1096" s="60" t="s">
+      <c r="D1096" s="32" t="s">
         <v>3404</v>
       </c>
-      <c r="E1096" s="60" t="s">
+      <c r="E1096" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="F1096" s="61"/>
-      <c r="G1096" s="60"/>
-      <c r="H1096" s="60"/>
-      <c r="I1096" s="60"/>
-      <c r="J1096" s="60"/>
-      <c r="K1096" s="60"/>
-      <c r="L1096" s="60"/>
-      <c r="M1096" s="60"/>
-      <c r="N1096" s="60"/>
-    </row>
-    <row r="1097" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1097" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1097" s="53" t="s">
         <v>2818</v>
       </c>
@@ -48655,23 +48521,14 @@
       <c r="C1097" s="44" t="s">
         <v>3040</v>
       </c>
-      <c r="D1097" s="60" t="s">
+      <c r="D1097" s="32" t="s">
         <v>2715</v>
       </c>
-      <c r="E1097" s="60" t="s">
+      <c r="E1097" s="32" t="s">
         <v>857</v>
       </c>
-      <c r="F1097" s="61"/>
-      <c r="G1097" s="60"/>
-      <c r="H1097" s="60"/>
-      <c r="I1097" s="60"/>
-      <c r="J1097" s="60"/>
-      <c r="K1097" s="60"/>
-      <c r="L1097" s="60"/>
-      <c r="M1097" s="60"/>
-      <c r="N1097" s="60"/>
-    </row>
-    <row r="1098" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1098" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1098" s="53" t="s">
         <v>2768</v>
       </c>
@@ -48681,23 +48538,14 @@
       <c r="C1098" s="44" t="s">
         <v>2990</v>
       </c>
-      <c r="D1098" s="60" t="s">
+      <c r="D1098" s="32" t="s">
         <v>2715</v>
       </c>
-      <c r="E1098" s="60" t="s">
+      <c r="E1098" s="32" t="s">
         <v>3416</v>
       </c>
-      <c r="F1098" s="61"/>
-      <c r="G1098" s="60"/>
-      <c r="H1098" s="60"/>
-      <c r="I1098" s="60"/>
-      <c r="J1098" s="60"/>
-      <c r="K1098" s="60"/>
-      <c r="L1098" s="60"/>
-      <c r="M1098" s="60"/>
-      <c r="N1098" s="60"/>
-    </row>
-    <row r="1099" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1099" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1099" s="53" t="s">
         <v>2800</v>
       </c>
@@ -48707,23 +48555,14 @@
       <c r="C1099" s="44" t="s">
         <v>3022</v>
       </c>
-      <c r="D1099" s="60" t="s">
+      <c r="D1099" s="32" t="s">
         <v>3410</v>
       </c>
-      <c r="E1099" s="60" t="s">
+      <c r="E1099" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="F1099" s="61"/>
-      <c r="G1099" s="60"/>
-      <c r="H1099" s="60"/>
-      <c r="I1099" s="60"/>
-      <c r="J1099" s="60"/>
-      <c r="K1099" s="60"/>
-      <c r="L1099" s="60"/>
-      <c r="M1099" s="60"/>
-      <c r="N1099" s="60"/>
-    </row>
-    <row r="1100" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1100" s="53" t="s">
         <v>2731</v>
       </c>
@@ -48733,23 +48572,14 @@
       <c r="C1100" s="44" t="s">
         <v>2953</v>
       </c>
-      <c r="D1100" s="60" t="s">
+      <c r="D1100" s="32" t="s">
         <v>3392</v>
       </c>
-      <c r="E1100" s="60" t="s">
+      <c r="E1100" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="F1100" s="61"/>
-      <c r="G1100" s="60"/>
-      <c r="H1100" s="60"/>
-      <c r="I1100" s="60"/>
-      <c r="J1100" s="60"/>
-      <c r="K1100" s="60"/>
-      <c r="L1100" s="60"/>
-      <c r="M1100" s="60"/>
-      <c r="N1100" s="60"/>
-    </row>
-    <row r="1101" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1101" s="53" t="s">
         <v>2730</v>
       </c>
@@ -48759,23 +48589,14 @@
       <c r="C1101" s="44" t="s">
         <v>2952</v>
       </c>
-      <c r="D1101" s="60" t="s">
+      <c r="D1101" s="32" t="s">
         <v>3392</v>
       </c>
-      <c r="E1101" s="60" t="s">
+      <c r="E1101" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="F1101" s="61"/>
-      <c r="G1101" s="60"/>
-      <c r="H1101" s="60"/>
-      <c r="I1101" s="60"/>
-      <c r="J1101" s="60"/>
-      <c r="K1101" s="60"/>
-      <c r="L1101" s="60"/>
-      <c r="M1101" s="60"/>
-      <c r="N1101" s="60"/>
-    </row>
-    <row r="1102" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1102" s="53" t="s">
         <v>2844</v>
       </c>
@@ -48785,27 +48606,20 @@
       <c r="C1102" s="44" t="s">
         <v>3066</v>
       </c>
-      <c r="D1102" s="60" t="s">
+      <c r="D1102" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="E1102" s="60" t="s">
+      <c r="E1102" s="32" t="s">
         <v>366</v>
       </c>
-      <c r="F1102" s="61"/>
-      <c r="G1102" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="H1102" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="I1102" s="60"/>
-      <c r="J1102" s="60"/>
-      <c r="K1102" s="60"/>
-      <c r="L1102" s="60"/>
-      <c r="M1102" s="60"/>
-      <c r="N1102" s="60"/>
-    </row>
-    <row r="1103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G1102" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1102" s="32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1103" s="53" t="s">
         <v>2754</v>
       </c>
@@ -48815,27 +48629,20 @@
       <c r="C1103" s="44" t="s">
         <v>2976</v>
       </c>
-      <c r="D1103" s="60" t="s">
+      <c r="D1103" s="32" t="s">
         <v>3375</v>
       </c>
-      <c r="E1103" s="60" t="s">
+      <c r="E1103" s="32" t="s">
         <v>366</v>
       </c>
-      <c r="F1103" s="61"/>
-      <c r="G1103" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="H1103" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="I1103" s="60"/>
-      <c r="J1103" s="60"/>
-      <c r="K1103" s="60"/>
-      <c r="L1103" s="60"/>
-      <c r="M1103" s="60"/>
-      <c r="N1103" s="60"/>
-    </row>
-    <row r="1104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G1103" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1103" s="32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1104" s="53" t="s">
         <v>2786</v>
       </c>
@@ -48845,27 +48652,20 @@
       <c r="C1104" s="44" t="s">
         <v>3008</v>
       </c>
-      <c r="D1104" s="60" t="s">
+      <c r="D1104" s="32" t="s">
         <v>315</v>
       </c>
-      <c r="E1104" s="60" t="s">
+      <c r="E1104" s="32" t="s">
         <v>366</v>
       </c>
-      <c r="F1104" s="61"/>
-      <c r="G1104" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="H1104" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="I1104" s="60"/>
-      <c r="J1104" s="60"/>
-      <c r="K1104" s="60"/>
-      <c r="L1104" s="60"/>
-      <c r="M1104" s="60"/>
-      <c r="N1104" s="60"/>
-    </row>
-    <row r="1105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G1104" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1104" s="32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1105" s="53" t="s">
         <v>2814</v>
       </c>
@@ -48875,27 +48675,20 @@
       <c r="C1105" s="44" t="s">
         <v>3036</v>
       </c>
-      <c r="D1105" s="60" t="s">
+      <c r="D1105" s="32" t="s">
         <v>315</v>
       </c>
-      <c r="E1105" s="60" t="s">
+      <c r="E1105" s="32" t="s">
         <v>366</v>
       </c>
-      <c r="F1105" s="61"/>
-      <c r="G1105" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="H1105" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="I1105" s="60"/>
-      <c r="J1105" s="60"/>
-      <c r="K1105" s="60"/>
-      <c r="L1105" s="60"/>
-      <c r="M1105" s="60"/>
-      <c r="N1105" s="60"/>
-    </row>
-    <row r="1106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G1105" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1105" s="32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1106" s="53" t="s">
         <v>2896</v>
       </c>
@@ -48905,23 +48698,14 @@
       <c r="C1106" s="44" t="s">
         <v>3100</v>
       </c>
-      <c r="D1106" s="60" t="s">
+      <c r="D1106" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="E1106" s="60" t="s">
+      <c r="E1106" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="F1106" s="61"/>
-      <c r="G1106" s="60"/>
-      <c r="H1106" s="60"/>
-      <c r="I1106" s="60"/>
-      <c r="J1106" s="60"/>
-      <c r="K1106" s="60"/>
-      <c r="L1106" s="60"/>
-      <c r="M1106" s="60"/>
-      <c r="N1106" s="60"/>
-    </row>
-    <row r="1107" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1107" s="53" t="s">
         <v>3487</v>
       </c>
@@ -48931,21 +48715,11 @@
       <c r="C1107" s="44" t="s">
         <v>3489</v>
       </c>
-      <c r="D1107" s="60" t="s">
+      <c r="D1107" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="E1107" s="60"/>
-      <c r="F1107" s="61"/>
-      <c r="G1107" s="60"/>
-      <c r="H1107" s="60"/>
-      <c r="I1107" s="60"/>
-      <c r="J1107" s="60"/>
-      <c r="K1107" s="60"/>
-      <c r="L1107" s="60"/>
-      <c r="M1107" s="60"/>
-      <c r="N1107" s="60"/>
-    </row>
-    <row r="1108" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1108" s="53" t="s">
         <v>3484</v>
       </c>
@@ -48955,21 +48729,11 @@
       <c r="C1108" s="44" t="s">
         <v>3485</v>
       </c>
-      <c r="D1108" s="60" t="s">
+      <c r="D1108" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="E1108" s="60"/>
-      <c r="F1108" s="61"/>
-      <c r="G1108" s="60"/>
-      <c r="H1108" s="60"/>
-      <c r="I1108" s="60"/>
-      <c r="J1108" s="60"/>
-      <c r="K1108" s="60"/>
-      <c r="L1108" s="60"/>
-      <c r="M1108" s="60"/>
-      <c r="N1108" s="60"/>
-    </row>
-    <row r="1109" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1109" s="53" t="s">
         <v>3466</v>
       </c>
@@ -48979,21 +48743,11 @@
       <c r="C1109" s="44" t="s">
         <v>3468</v>
       </c>
-      <c r="D1109" s="60" t="s">
+      <c r="D1109" s="32" t="s">
         <v>3469</v>
       </c>
-      <c r="E1109" s="60"/>
-      <c r="F1109" s="61"/>
-      <c r="G1109" s="60"/>
-      <c r="H1109" s="60"/>
-      <c r="I1109" s="60"/>
-      <c r="J1109" s="60"/>
-      <c r="K1109" s="60"/>
-      <c r="L1109" s="60"/>
-      <c r="M1109" s="60"/>
-      <c r="N1109" s="60"/>
-    </row>
-    <row r="1110" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1110" s="53" t="s">
         <v>3470</v>
       </c>
@@ -49003,21 +48757,11 @@
       <c r="C1110" s="44" t="s">
         <v>3472</v>
       </c>
-      <c r="D1110" s="60" t="s">
+      <c r="D1110" s="32" t="s">
         <v>3469</v>
       </c>
-      <c r="E1110" s="60"/>
-      <c r="F1110" s="61"/>
-      <c r="G1110" s="60"/>
-      <c r="H1110" s="60"/>
-      <c r="I1110" s="60"/>
-      <c r="J1110" s="60"/>
-      <c r="K1110" s="60"/>
-      <c r="L1110" s="60"/>
-      <c r="M1110" s="60"/>
-      <c r="N1110" s="60"/>
-    </row>
-    <row r="1111" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1111" s="53" t="s">
         <v>3462</v>
       </c>
@@ -49027,21 +48771,11 @@
       <c r="C1111" s="44" t="s">
         <v>3464</v>
       </c>
-      <c r="D1111" s="60" t="s">
+      <c r="D1111" s="32" t="s">
         <v>3465</v>
       </c>
-      <c r="E1111" s="60"/>
-      <c r="F1111" s="61"/>
-      <c r="G1111" s="60"/>
-      <c r="H1111" s="60"/>
-      <c r="I1111" s="60"/>
-      <c r="J1111" s="60"/>
-      <c r="K1111" s="60"/>
-      <c r="L1111" s="60"/>
-      <c r="M1111" s="60"/>
-      <c r="N1111" s="60"/>
-    </row>
-    <row r="1112" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1112" s="53" t="s">
         <v>3593</v>
       </c>
@@ -49051,21 +48785,11 @@
       <c r="C1112" s="44" t="s">
         <v>3591</v>
       </c>
-      <c r="D1112" s="60" t="s">
+      <c r="D1112" s="32" t="s">
         <v>3595</v>
       </c>
-      <c r="E1112" s="60"/>
-      <c r="F1112" s="61"/>
-      <c r="G1112" s="60"/>
-      <c r="H1112" s="60"/>
-      <c r="I1112" s="60"/>
-      <c r="J1112" s="60"/>
-      <c r="K1112" s="60"/>
-      <c r="L1112" s="60"/>
-      <c r="M1112" s="60"/>
-      <c r="N1112" s="60"/>
-    </row>
-    <row r="1113" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1113" s="53" t="s">
         <v>3459</v>
       </c>
@@ -49075,21 +48799,11 @@
       <c r="C1113" s="44" t="s">
         <v>3461</v>
       </c>
-      <c r="D1113" s="60" t="s">
+      <c r="D1113" s="32" t="s">
         <v>3403</v>
       </c>
-      <c r="E1113" s="60"/>
-      <c r="F1113" s="61"/>
-      <c r="G1113" s="60"/>
-      <c r="H1113" s="60"/>
-      <c r="I1113" s="60"/>
-      <c r="J1113" s="60"/>
-      <c r="K1113" s="60"/>
-      <c r="L1113" s="60"/>
-      <c r="M1113" s="60"/>
-      <c r="N1113" s="60"/>
-    </row>
-    <row r="1114" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1114" s="53" t="s">
         <v>3478</v>
       </c>
@@ -49099,21 +48813,11 @@
       <c r="C1114" s="44" t="s">
         <v>3480</v>
       </c>
-      <c r="D1114" s="60" t="s">
+      <c r="D1114" s="32" t="s">
         <v>627</v>
       </c>
-      <c r="E1114" s="60"/>
-      <c r="F1114" s="61"/>
-      <c r="G1114" s="60"/>
-      <c r="H1114" s="60"/>
-      <c r="I1114" s="60"/>
-      <c r="J1114" s="60"/>
-      <c r="K1114" s="60"/>
-      <c r="L1114" s="60"/>
-      <c r="M1114" s="60"/>
-      <c r="N1114" s="60"/>
-    </row>
-    <row r="1115" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1115" s="53" t="s">
         <v>3711</v>
       </c>
@@ -49123,21 +48827,11 @@
       <c r="C1115" s="44" t="s">
         <v>3475</v>
       </c>
-      <c r="D1115" s="60" t="s">
+      <c r="D1115" s="32" t="s">
         <v>3476</v>
       </c>
-      <c r="E1115" s="60"/>
-      <c r="F1115" s="61"/>
-      <c r="G1115" s="60"/>
-      <c r="H1115" s="60"/>
-      <c r="I1115" s="60"/>
-      <c r="J1115" s="60"/>
-      <c r="K1115" s="60"/>
-      <c r="L1115" s="60"/>
-      <c r="M1115" s="60"/>
-      <c r="N1115" s="60"/>
-    </row>
-    <row r="1116" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1116" s="53" t="s">
         <v>3510</v>
       </c>
@@ -49147,21 +48841,11 @@
       <c r="C1116" s="44" t="s">
         <v>3512</v>
       </c>
-      <c r="D1116" s="60" t="s">
+      <c r="D1116" s="32" t="s">
         <v>3513</v>
       </c>
-      <c r="E1116" s="60"/>
-      <c r="F1116" s="61"/>
-      <c r="G1116" s="60"/>
-      <c r="H1116" s="60"/>
-      <c r="I1116" s="60"/>
-      <c r="J1116" s="60"/>
-      <c r="K1116" s="60"/>
-      <c r="L1116" s="60"/>
-      <c r="M1116" s="60"/>
-      <c r="N1116" s="60"/>
-    </row>
-    <row r="1117" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1117" s="53" t="s">
         <v>3491</v>
       </c>
@@ -49171,21 +48855,11 @@
       <c r="C1117" s="44" t="s">
         <v>3492</v>
       </c>
-      <c r="D1117" s="60" t="s">
+      <c r="D1117" s="32" t="s">
         <v>3403</v>
       </c>
-      <c r="E1117" s="60"/>
-      <c r="F1117" s="61"/>
-      <c r="G1117" s="60"/>
-      <c r="H1117" s="60"/>
-      <c r="I1117" s="60"/>
-      <c r="J1117" s="60"/>
-      <c r="K1117" s="60"/>
-      <c r="L1117" s="60"/>
-      <c r="M1117" s="60"/>
-      <c r="N1117" s="60"/>
-    </row>
-    <row r="1118" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1118" s="53" t="s">
         <v>3644</v>
       </c>
@@ -49195,21 +48869,11 @@
       <c r="C1118" s="44" t="s">
         <v>3646</v>
       </c>
-      <c r="D1118" s="60" t="s">
+      <c r="D1118" s="32" t="s">
         <v>3647</v>
       </c>
-      <c r="E1118" s="60"/>
-      <c r="F1118" s="61"/>
-      <c r="G1118" s="60"/>
-      <c r="H1118" s="60"/>
-      <c r="I1118" s="60"/>
-      <c r="J1118" s="60"/>
-      <c r="K1118" s="60"/>
-      <c r="L1118" s="60"/>
-      <c r="M1118" s="60"/>
-      <c r="N1118" s="60"/>
-    </row>
-    <row r="1119" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1119" s="53" t="s">
         <v>3530</v>
       </c>
@@ -49219,21 +48883,11 @@
       <c r="C1119" s="44" t="s">
         <v>3532</v>
       </c>
-      <c r="D1119" s="60" t="s">
+      <c r="D1119" s="32" t="s">
         <v>3533</v>
       </c>
-      <c r="E1119" s="60"/>
-      <c r="F1119" s="61"/>
-      <c r="G1119" s="60"/>
-      <c r="H1119" s="60"/>
-      <c r="I1119" s="60"/>
-      <c r="J1119" s="60"/>
-      <c r="K1119" s="60"/>
-      <c r="L1119" s="60"/>
-      <c r="M1119" s="60"/>
-      <c r="N1119" s="60"/>
-    </row>
-    <row r="1120" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1120" s="53" t="s">
         <v>3680</v>
       </c>
@@ -49243,21 +48897,11 @@
       <c r="C1120" s="44" t="s">
         <v>3682</v>
       </c>
-      <c r="D1120" s="60" t="s">
+      <c r="D1120" s="32" t="s">
         <v>315</v>
       </c>
-      <c r="E1120" s="60"/>
-      <c r="F1120" s="61"/>
-      <c r="G1120" s="60"/>
-      <c r="H1120" s="60"/>
-      <c r="I1120" s="60"/>
-      <c r="J1120" s="60"/>
-      <c r="K1120" s="60"/>
-      <c r="L1120" s="60"/>
-      <c r="M1120" s="60"/>
-      <c r="N1120" s="60"/>
-    </row>
-    <row r="1121" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1121" s="53" t="s">
         <v>3623</v>
       </c>
@@ -49267,21 +48911,11 @@
       <c r="C1121" s="44" t="s">
         <v>3625</v>
       </c>
-      <c r="D1121" s="60" t="s">
+      <c r="D1121" s="32" t="s">
         <v>3626</v>
       </c>
-      <c r="E1121" s="60"/>
-      <c r="F1121" s="61"/>
-      <c r="G1121" s="60"/>
-      <c r="H1121" s="60"/>
-      <c r="I1121" s="60"/>
-      <c r="J1121" s="60"/>
-      <c r="K1121" s="60"/>
-      <c r="L1121" s="60"/>
-      <c r="M1121" s="60"/>
-      <c r="N1121" s="60"/>
-    </row>
-    <row r="1122" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1122" s="55" t="s">
         <v>3650</v>
       </c>
@@ -49294,18 +48928,8 @@
       <c r="D1122" s="35" t="s">
         <v>3653</v>
       </c>
-      <c r="E1122" s="60"/>
-      <c r="F1122" s="61"/>
-      <c r="G1122" s="60"/>
-      <c r="H1122" s="60"/>
-      <c r="I1122" s="60"/>
-      <c r="J1122" s="60"/>
-      <c r="K1122" s="60"/>
-      <c r="L1122" s="60"/>
-      <c r="M1122" s="60"/>
-      <c r="N1122" s="60"/>
-    </row>
-    <row r="1123" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1123" s="53" t="s">
         <v>3545</v>
       </c>
@@ -49315,21 +48939,11 @@
       <c r="C1123" s="44" t="s">
         <v>3540</v>
       </c>
-      <c r="D1123" s="60" t="s">
+      <c r="D1123" s="32" t="s">
         <v>3547</v>
       </c>
-      <c r="E1123" s="60"/>
-      <c r="F1123" s="61"/>
-      <c r="G1123" s="60"/>
-      <c r="H1123" s="60"/>
-      <c r="I1123" s="60"/>
-      <c r="J1123" s="60"/>
-      <c r="K1123" s="60"/>
-      <c r="L1123" s="60"/>
-      <c r="M1123" s="60"/>
-      <c r="N1123" s="60"/>
-    </row>
-    <row r="1124" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1124" s="53" t="s">
         <v>3612</v>
       </c>
@@ -49339,21 +48953,11 @@
       <c r="C1124" s="44" t="s">
         <v>3614</v>
       </c>
-      <c r="D1124" s="60" t="s">
+      <c r="D1124" s="32" t="s">
         <v>3611</v>
       </c>
-      <c r="E1124" s="60"/>
-      <c r="F1124" s="61"/>
-      <c r="G1124" s="60"/>
-      <c r="H1124" s="60"/>
-      <c r="I1124" s="60"/>
-      <c r="J1124" s="60"/>
-      <c r="K1124" s="60"/>
-      <c r="L1124" s="60"/>
-      <c r="M1124" s="60"/>
-      <c r="N1124" s="60"/>
-    </row>
-    <row r="1125" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1125" s="53" t="s">
         <v>3608</v>
       </c>
@@ -49363,21 +48967,11 @@
       <c r="C1125" s="44" t="s">
         <v>3610</v>
       </c>
-      <c r="D1125" s="60" t="s">
+      <c r="D1125" s="32" t="s">
         <v>3611</v>
       </c>
-      <c r="E1125" s="60"/>
-      <c r="F1125" s="61"/>
-      <c r="G1125" s="60"/>
-      <c r="H1125" s="60"/>
-      <c r="I1125" s="60"/>
-      <c r="J1125" s="60"/>
-      <c r="K1125" s="60"/>
-      <c r="L1125" s="60"/>
-      <c r="M1125" s="60"/>
-      <c r="N1125" s="60"/>
-    </row>
-    <row r="1126" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1126" s="53" t="s">
         <v>3599</v>
       </c>
@@ -49387,21 +48981,11 @@
       <c r="C1126" s="44" t="s">
         <v>3598</v>
       </c>
-      <c r="D1126" s="60" t="s">
+      <c r="D1126" s="32" t="s">
         <v>3537</v>
       </c>
-      <c r="E1126" s="60"/>
-      <c r="F1126" s="61"/>
-      <c r="G1126" s="60"/>
-      <c r="H1126" s="60"/>
-      <c r="I1126" s="60"/>
-      <c r="J1126" s="60"/>
-      <c r="K1126" s="60"/>
-      <c r="L1126" s="60"/>
-      <c r="M1126" s="60"/>
-      <c r="N1126" s="60"/>
-    </row>
-    <row r="1127" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1127" s="53" t="s">
         <v>3534</v>
       </c>
@@ -49414,18 +48998,8 @@
       <c r="D1127" s="35" t="s">
         <v>3537</v>
       </c>
-      <c r="E1127" s="60"/>
-      <c r="F1127" s="61"/>
-      <c r="G1127" s="60"/>
-      <c r="H1127" s="60"/>
-      <c r="I1127" s="60"/>
-      <c r="J1127" s="60"/>
-      <c r="K1127" s="60"/>
-      <c r="L1127" s="60"/>
-      <c r="M1127" s="60"/>
-      <c r="N1127" s="60"/>
-    </row>
-    <row r="1128" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1128" s="53" t="s">
         <v>3596</v>
       </c>
@@ -49438,18 +49012,8 @@
       <c r="D1128" s="54" t="s">
         <v>245</v>
       </c>
-      <c r="E1128" s="60"/>
-      <c r="F1128" s="61"/>
-      <c r="G1128" s="60"/>
-      <c r="H1128" s="60"/>
-      <c r="I1128" s="60"/>
-      <c r="J1128" s="60"/>
-      <c r="K1128" s="60"/>
-      <c r="L1128" s="60"/>
-      <c r="M1128" s="60"/>
-      <c r="N1128" s="60"/>
-    </row>
-    <row r="1129" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1129" s="53" t="s">
         <v>3693</v>
       </c>
@@ -49459,21 +49023,11 @@
       <c r="C1129" s="44" t="s">
         <v>3685</v>
       </c>
-      <c r="D1129" s="60" t="s">
+      <c r="D1129" s="32" t="s">
         <v>3695</v>
       </c>
-      <c r="E1129" s="60"/>
-      <c r="F1129" s="61"/>
-      <c r="G1129" s="60"/>
-      <c r="H1129" s="60"/>
-      <c r="I1129" s="60"/>
-      <c r="J1129" s="60"/>
-      <c r="K1129" s="60"/>
-      <c r="L1129" s="60"/>
-      <c r="M1129" s="60"/>
-      <c r="N1129" s="60"/>
-    </row>
-    <row r="1130" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1130" s="53" t="s">
         <v>3516</v>
       </c>
@@ -49483,21 +49037,11 @@
       <c r="C1130" s="44" t="s">
         <v>3550</v>
       </c>
-      <c r="D1130" s="60" t="s">
+      <c r="D1130" s="32" t="s">
         <v>3518</v>
       </c>
-      <c r="E1130" s="60"/>
-      <c r="F1130" s="61"/>
-      <c r="G1130" s="60"/>
-      <c r="H1130" s="60"/>
-      <c r="I1130" s="60"/>
-      <c r="J1130" s="60"/>
-      <c r="K1130" s="60"/>
-      <c r="L1130" s="60"/>
-      <c r="M1130" s="60"/>
-      <c r="N1130" s="60"/>
-    </row>
-    <row r="1131" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1131" s="53" t="s">
         <v>3630</v>
       </c>
@@ -49507,21 +49051,11 @@
       <c r="C1131" s="44" t="s">
         <v>3598</v>
       </c>
-      <c r="D1131" s="60" t="s">
+      <c r="D1131" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="E1131" s="60"/>
-      <c r="F1131" s="61"/>
-      <c r="G1131" s="60"/>
-      <c r="H1131" s="60"/>
-      <c r="I1131" s="60"/>
-      <c r="J1131" s="60"/>
-      <c r="K1131" s="60"/>
-      <c r="L1131" s="60"/>
-      <c r="M1131" s="60"/>
-      <c r="N1131" s="60"/>
-    </row>
-    <row r="1132" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1132" s="53" t="s">
         <v>3632</v>
       </c>
@@ -49531,21 +49065,11 @@
       <c r="C1132" s="44" t="s">
         <v>3536</v>
       </c>
-      <c r="D1132" s="60" t="s">
+      <c r="D1132" s="32" t="s">
         <v>3695</v>
       </c>
-      <c r="E1132" s="60"/>
-      <c r="F1132" s="61"/>
-      <c r="G1132" s="60"/>
-      <c r="H1132" s="60"/>
-      <c r="I1132" s="60"/>
-      <c r="J1132" s="60"/>
-      <c r="K1132" s="60"/>
-      <c r="L1132" s="60"/>
-      <c r="M1132" s="60"/>
-      <c r="N1132" s="60"/>
-    </row>
-    <row r="1133" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1133" s="53" t="s">
         <v>3683</v>
       </c>
@@ -49555,21 +49079,11 @@
       <c r="C1133" s="44" t="s">
         <v>3685</v>
       </c>
-      <c r="D1133" s="60" t="s">
+      <c r="D1133" s="32" t="s">
         <v>3686</v>
       </c>
-      <c r="E1133" s="60"/>
-      <c r="F1133" s="61"/>
-      <c r="G1133" s="60"/>
-      <c r="H1133" s="60"/>
-      <c r="I1133" s="60"/>
-      <c r="J1133" s="60"/>
-      <c r="K1133" s="60"/>
-      <c r="L1133" s="60"/>
-      <c r="M1133" s="60"/>
-      <c r="N1133" s="60"/>
-    </row>
-    <row r="1134" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1134" s="53" t="s">
         <v>3507</v>
       </c>
@@ -49579,21 +49093,11 @@
       <c r="C1134" s="44" t="s">
         <v>3549</v>
       </c>
-      <c r="D1134" s="60" t="s">
+      <c r="D1134" s="32" t="s">
         <v>3509</v>
       </c>
-      <c r="E1134" s="60"/>
-      <c r="F1134" s="61"/>
-      <c r="G1134" s="60"/>
-      <c r="H1134" s="60"/>
-      <c r="I1134" s="60"/>
-      <c r="J1134" s="60"/>
-      <c r="K1134" s="60"/>
-      <c r="L1134" s="60"/>
-      <c r="M1134" s="60"/>
-      <c r="N1134" s="60"/>
-    </row>
-    <row r="1135" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1135" s="53" t="s">
         <v>3569</v>
       </c>
@@ -49603,21 +49107,11 @@
       <c r="C1135" s="44" t="s">
         <v>3571</v>
       </c>
-      <c r="D1135" s="60" t="s">
+      <c r="D1135" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="E1135" s="60"/>
-      <c r="F1135" s="61"/>
-      <c r="G1135" s="60"/>
-      <c r="H1135" s="60"/>
-      <c r="I1135" s="60"/>
-      <c r="J1135" s="60"/>
-      <c r="K1135" s="60"/>
-      <c r="L1135" s="60"/>
-      <c r="M1135" s="60"/>
-      <c r="N1135" s="60"/>
-    </row>
-    <row r="1136" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1136" s="53" t="s">
         <v>3566</v>
       </c>
@@ -49627,21 +49121,11 @@
       <c r="C1136" s="44" t="s">
         <v>3568</v>
       </c>
-      <c r="D1136" s="60" t="s">
+      <c r="D1136" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="E1136" s="60"/>
-      <c r="F1136" s="61"/>
-      <c r="G1136" s="60"/>
-      <c r="H1136" s="60"/>
-      <c r="I1136" s="60"/>
-      <c r="J1136" s="60"/>
-      <c r="K1136" s="60"/>
-      <c r="L1136" s="60"/>
-      <c r="M1136" s="60"/>
-      <c r="N1136" s="60"/>
-    </row>
-    <row r="1137" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1137" s="53" t="s">
         <v>3577</v>
       </c>
@@ -49651,21 +49135,11 @@
       <c r="C1137" s="44" t="s">
         <v>3536</v>
       </c>
-      <c r="D1137" s="60" t="s">
+      <c r="D1137" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="E1137" s="60"/>
-      <c r="F1137" s="61"/>
-      <c r="G1137" s="60"/>
-      <c r="H1137" s="60"/>
-      <c r="I1137" s="60"/>
-      <c r="J1137" s="60"/>
-      <c r="K1137" s="60"/>
-      <c r="L1137" s="60"/>
-      <c r="M1137" s="60"/>
-      <c r="N1137" s="60"/>
-    </row>
-    <row r="1138" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1138" s="53" t="s">
         <v>3705</v>
       </c>
@@ -49675,21 +49149,11 @@
       <c r="C1138" s="44" t="s">
         <v>3703</v>
       </c>
-      <c r="D1138" s="60" t="s">
+      <c r="D1138" s="32" t="s">
         <v>3702</v>
       </c>
-      <c r="E1138" s="60"/>
-      <c r="F1138" s="61"/>
-      <c r="G1138" s="60"/>
-      <c r="H1138" s="60"/>
-      <c r="I1138" s="60"/>
-      <c r="J1138" s="60"/>
-      <c r="K1138" s="60"/>
-      <c r="L1138" s="60"/>
-      <c r="M1138" s="60"/>
-      <c r="N1138" s="60"/>
-    </row>
-    <row r="1139" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1139" s="53" t="s">
         <v>3699</v>
       </c>
@@ -49699,21 +49163,11 @@
       <c r="C1139" s="44" t="s">
         <v>3701</v>
       </c>
-      <c r="D1139" s="60" t="s">
+      <c r="D1139" s="32" t="s">
         <v>3702</v>
       </c>
-      <c r="E1139" s="60"/>
-      <c r="F1139" s="61"/>
-      <c r="G1139" s="60"/>
-      <c r="H1139" s="60"/>
-      <c r="I1139" s="60"/>
-      <c r="J1139" s="60"/>
-      <c r="K1139" s="60"/>
-      <c r="L1139" s="60"/>
-      <c r="M1139" s="60"/>
-      <c r="N1139" s="60"/>
-    </row>
-    <row r="1140" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1140" s="53" t="s">
         <v>3555</v>
       </c>
@@ -49723,21 +49177,11 @@
       <c r="C1140" s="44" t="s">
         <v>3557</v>
       </c>
-      <c r="D1140" s="60" t="s">
+      <c r="D1140" s="32" t="s">
         <v>3558</v>
       </c>
-      <c r="E1140" s="60"/>
-      <c r="F1140" s="61"/>
-      <c r="G1140" s="60"/>
-      <c r="H1140" s="60"/>
-      <c r="I1140" s="60"/>
-      <c r="J1140" s="60"/>
-      <c r="K1140" s="60"/>
-      <c r="L1140" s="60"/>
-      <c r="M1140" s="60"/>
-      <c r="N1140" s="60"/>
-    </row>
-    <row r="1141" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1141" s="59" t="s">
         <v>3627</v>
       </c>
@@ -49750,18 +49194,8 @@
       <c r="D1141" s="55" t="s">
         <v>3672</v>
       </c>
-      <c r="E1141" s="60"/>
-      <c r="F1141" s="61"/>
-      <c r="G1141" s="60"/>
-      <c r="H1141" s="60"/>
-      <c r="I1141" s="60"/>
-      <c r="J1141" s="60"/>
-      <c r="K1141" s="60"/>
-      <c r="L1141" s="60"/>
-      <c r="M1141" s="60"/>
-      <c r="N1141" s="60"/>
-    </row>
-    <row r="1142" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1142" s="53" t="s">
         <v>3673</v>
       </c>
@@ -49771,21 +49205,11 @@
       <c r="C1142" s="44" t="s">
         <v>3591</v>
       </c>
-      <c r="D1142" s="60" t="s">
+      <c r="D1142" s="32" t="s">
         <v>3675</v>
       </c>
-      <c r="E1142" s="60"/>
-      <c r="F1142" s="61"/>
-      <c r="G1142" s="60"/>
-      <c r="H1142" s="60"/>
-      <c r="I1142" s="60"/>
-      <c r="J1142" s="60"/>
-      <c r="K1142" s="60"/>
-      <c r="L1142" s="60"/>
-      <c r="M1142" s="60"/>
-      <c r="N1142" s="60"/>
-    </row>
-    <row r="1143" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1143" s="53" t="s">
         <v>3690</v>
       </c>
@@ -49795,21 +49219,11 @@
       <c r="C1143" s="44" t="s">
         <v>3692</v>
       </c>
-      <c r="D1143" s="60" t="s">
+      <c r="D1143" s="32" t="s">
         <v>3672</v>
       </c>
-      <c r="E1143" s="60"/>
-      <c r="F1143" s="61"/>
-      <c r="G1143" s="60"/>
-      <c r="H1143" s="60"/>
-      <c r="I1143" s="60"/>
-      <c r="J1143" s="60"/>
-      <c r="K1143" s="60"/>
-      <c r="L1143" s="60"/>
-      <c r="M1143" s="60"/>
-      <c r="N1143" s="60"/>
-    </row>
-    <row r="1144" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1144" s="53" t="s">
         <v>3522</v>
       </c>
@@ -49819,21 +49233,11 @@
       <c r="C1144" s="44" t="s">
         <v>3524</v>
       </c>
-      <c r="D1144" s="60" t="s">
+      <c r="D1144" s="32" t="s">
         <v>3525</v>
       </c>
-      <c r="E1144" s="60"/>
-      <c r="F1144" s="61"/>
-      <c r="G1144" s="60"/>
-      <c r="H1144" s="60"/>
-      <c r="I1144" s="60"/>
-      <c r="J1144" s="60"/>
-      <c r="K1144" s="60"/>
-      <c r="L1144" s="60"/>
-      <c r="M1144" s="60"/>
-      <c r="N1144" s="60"/>
-    </row>
-    <row r="1145" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1145" s="53" t="s">
         <v>3619</v>
       </c>
@@ -49843,21 +49247,11 @@
       <c r="C1145" s="44" t="s">
         <v>3621</v>
       </c>
-      <c r="D1145" s="60" t="s">
+      <c r="D1145" s="32" t="s">
         <v>3622</v>
       </c>
-      <c r="E1145" s="60"/>
-      <c r="F1145" s="61"/>
-      <c r="G1145" s="60"/>
-      <c r="H1145" s="60"/>
-      <c r="I1145" s="60"/>
-      <c r="J1145" s="60"/>
-      <c r="K1145" s="60"/>
-      <c r="L1145" s="60"/>
-      <c r="M1145" s="60"/>
-      <c r="N1145" s="60"/>
-    </row>
-    <row r="1146" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1146" s="53" t="s">
         <v>3582</v>
       </c>
@@ -49867,21 +49261,11 @@
       <c r="C1146" s="44" t="s">
         <v>3584</v>
       </c>
-      <c r="D1146" s="60" t="s">
+      <c r="D1146" s="32" t="s">
         <v>3585</v>
       </c>
-      <c r="E1146" s="60"/>
-      <c r="F1146" s="61"/>
-      <c r="G1146" s="60"/>
-      <c r="H1146" s="60"/>
-      <c r="I1146" s="60"/>
-      <c r="J1146" s="60"/>
-      <c r="K1146" s="60"/>
-      <c r="L1146" s="60"/>
-      <c r="M1146" s="60"/>
-      <c r="N1146" s="60"/>
-    </row>
-    <row r="1147" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1147" s="53" t="s">
         <v>3551</v>
       </c>
@@ -49891,21 +49275,11 @@
       <c r="C1147" s="44" t="s">
         <v>3553</v>
       </c>
-      <c r="D1147" s="60" t="s">
+      <c r="D1147" s="32" t="s">
         <v>3554</v>
       </c>
-      <c r="E1147" s="60"/>
-      <c r="F1147" s="61"/>
-      <c r="G1147" s="60"/>
-      <c r="H1147" s="60"/>
-      <c r="I1147" s="60"/>
-      <c r="J1147" s="60"/>
-      <c r="K1147" s="60"/>
-      <c r="L1147" s="60"/>
-      <c r="M1147" s="60"/>
-      <c r="N1147" s="60"/>
-    </row>
-    <row r="1148" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1148" s="53" t="s">
         <v>3667</v>
       </c>
@@ -49915,21 +49289,11 @@
       <c r="C1148" s="44" t="s">
         <v>3669</v>
       </c>
-      <c r="D1148" s="60" t="s">
+      <c r="D1148" s="32" t="s">
         <v>3670</v>
       </c>
-      <c r="E1148" s="60"/>
-      <c r="F1148" s="61"/>
-      <c r="G1148" s="60"/>
-      <c r="H1148" s="60"/>
-      <c r="I1148" s="60"/>
-      <c r="J1148" s="60"/>
-      <c r="K1148" s="60"/>
-      <c r="L1148" s="60"/>
-      <c r="M1148" s="60"/>
-      <c r="N1148" s="60"/>
-    </row>
-    <row r="1149" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1149" s="53" t="s">
         <v>3601</v>
       </c>
@@ -49939,21 +49303,11 @@
       <c r="C1149" s="44" t="s">
         <v>3603</v>
       </c>
-      <c r="D1149" s="60" t="s">
+      <c r="D1149" s="32" t="s">
         <v>2715</v>
       </c>
-      <c r="E1149" s="60"/>
-      <c r="F1149" s="61"/>
-      <c r="G1149" s="60"/>
-      <c r="H1149" s="60"/>
-      <c r="I1149" s="60"/>
-      <c r="J1149" s="60"/>
-      <c r="K1149" s="60"/>
-      <c r="L1149" s="60"/>
-      <c r="M1149" s="60"/>
-      <c r="N1149" s="60"/>
-    </row>
-    <row r="1150" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1150" s="53" t="s">
         <v>3663</v>
       </c>
@@ -49963,75 +49317,53 @@
       <c r="C1150" s="44" t="s">
         <v>3560</v>
       </c>
-      <c r="D1150" s="60" t="s">
+      <c r="D1150" s="32" t="s">
         <v>517</v>
       </c>
-      <c r="E1150" s="60"/>
-      <c r="F1150" s="61"/>
-      <c r="G1150" s="60"/>
-      <c r="H1150" s="60"/>
-      <c r="I1150" s="60"/>
-      <c r="J1150" s="60"/>
-      <c r="K1150" s="60"/>
-      <c r="L1150" s="60"/>
-      <c r="M1150" s="60"/>
-      <c r="N1150" s="60"/>
-    </row>
-    <row r="1151" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1151" s="55"/>
       <c r="B1151" s="44"/>
       <c r="C1151" s="44" t="s">
         <v>2710</v>
       </c>
-      <c r="D1151" s="60" t="s">
+      <c r="D1151" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="E1151" s="60" t="s">
+      <c r="E1151" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="F1151" s="61" t="s">
+      <c r="F1151" s="52" t="s">
         <v>138</v>
       </c>
-      <c r="G1151" s="60"/>
-      <c r="H1151" s="60"/>
-      <c r="I1151" s="60" t="s">
-        <v>133</v>
-      </c>
-      <c r="J1151" s="60"/>
-      <c r="K1151" s="60"/>
-      <c r="L1151" s="60"/>
-      <c r="M1151" s="60"/>
-      <c r="N1151" s="60"/>
-    </row>
-    <row r="1152" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I1151" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1152" s="55"/>
       <c r="B1152" s="44"/>
       <c r="C1152" s="44" t="s">
         <v>2707</v>
       </c>
-      <c r="D1152" s="60" t="s">
+      <c r="D1152" s="32" t="s">
         <v>2708</v>
       </c>
-      <c r="E1152" s="60" t="s">
+      <c r="E1152" s="32" t="s">
         <v>416</v>
       </c>
-      <c r="F1152" s="61">
+      <c r="F1152" s="52">
         <v>4</v>
       </c>
-      <c r="G1152" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="H1152" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="I1152" s="60" t="s">
+      <c r="G1152" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1152" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1152" s="32" t="s">
         <v>2706</v>
       </c>
-      <c r="J1152" s="60"/>
-      <c r="K1152" s="60"/>
-      <c r="L1152" s="60"/>
-      <c r="M1152" s="60"/>
-      <c r="N1152" s="60"/>
     </row>
     <row r="1153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1153" s="55"/>
@@ -50046,11 +49378,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1153" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N1153">
-      <sortCondition ref="A1:A1153"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:O1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N1082">
     <sortCondition ref="D1:D1082"/>
   </sortState>

</xml_diff>

<commit_message>
Correct sales and bug fixes
</commit_message>
<xml_diff>
--- a/Database/Fabric_Work Order revise new.xlsx
+++ b/Database/Fabric_Work Order revise new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AadeshwarWorkOrder\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC16D06-C8F3-467E-9F81-E8ED69A37BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D5EAFD-6ADF-4C69-AFAA-653BED36C8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11818,9 +11818,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="78" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="78" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>